<commit_message>
Anpassungen Treffen Brixen 6.2.17
</commit_message>
<xml_diff>
--- a/2017 Reisen/TdF Bergisches Land/Kalkulation TdF.xlsx
+++ b/2017 Reisen/TdF Bergisches Land/Kalkulation TdF.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="47">
   <si>
     <t>Anzahl Nächte</t>
   </si>
@@ -153,6 +153,18 @@
   </si>
   <si>
     <t>Summe</t>
+  </si>
+  <si>
+    <t>Wo endet Gewinnzone?</t>
+  </si>
+  <si>
+    <t>Guide Trikot Pauschal</t>
+  </si>
+  <si>
+    <t>Guide Trikots</t>
+  </si>
+  <si>
+    <t>Guide pro Tag</t>
   </si>
 </sst>
 </file>
@@ -502,10 +514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -553,14 +565,14 @@
         <v>14</v>
       </c>
       <c r="E3" s="3">
-        <f>B17*(B9/2)*B1</f>
+        <f>B19*(B9/2)*B1</f>
         <v>6250</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H3" s="4">
-        <f>B17*B27</f>
+        <f>B19*B29</f>
         <v>15000</v>
       </c>
     </row>
@@ -575,14 +587,14 @@
         <v>13</v>
       </c>
       <c r="E4" s="3">
-        <f>B18*B10*B1</f>
+        <f>B20*B10*B1</f>
         <v>3465</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H4" s="4">
-        <f>B18*B28</f>
+        <f>B20*B30</f>
         <v>6510</v>
       </c>
     </row>
@@ -597,7 +609,7 @@
         <v>15</v>
       </c>
       <c r="E5" s="3">
-        <f>(B17+B18)*B11*B1</f>
+        <f>(B19+B20)*B11*B1</f>
         <v>4050</v>
       </c>
     </row>
@@ -658,8 +670,8 @@
         <v>16</v>
       </c>
       <c r="E9" s="3">
-        <f>125*B1</f>
-        <v>625</v>
+        <f>B16*(B4+B3)*B1</f>
+        <v>525</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -718,6 +730,13 @@
         <v>40</v>
       </c>
       <c r="C13" s="3"/>
+      <c r="D13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E13" s="3">
+        <f>B15*B21</f>
+        <v>135</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
@@ -731,7 +750,7 @@
       </c>
       <c r="E14" s="5">
         <f>SUM(E3:E13)</f>
-        <v>16110</v>
+        <v>16145</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2" t="s">
@@ -743,161 +762,190 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" s="8">
+        <v>5</v>
+      </c>
       <c r="D15" s="2"/>
       <c r="E15" s="5"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
-      <c r="H15" s="6"/>
+      <c r="H15" s="5"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" s="10">
-        <f>SUM(B3:B6)</f>
-        <v>3</v>
+      <c r="A16" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" s="8">
+        <v>35</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="5"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
-      <c r="H16" s="6"/>
+      <c r="H16" s="5"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" s="10">
-        <f>B7-B5-B3</f>
-        <v>20</v>
-      </c>
       <c r="D17" s="2"/>
       <c r="E17" s="5"/>
       <c r="F17" s="2"/>
-      <c r="G17" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="H17" s="6">
-        <f>H14-E14</f>
-        <v>5400</v>
-      </c>
+      <c r="G17" s="2"/>
+      <c r="H17" s="6"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="10" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="B18" s="10">
-        <f>B8-B6-B4</f>
-        <v>7</v>
+        <f>SUM(B3:B6)</f>
+        <v>3</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="5"/>
       <c r="F18" s="2"/>
-      <c r="G18" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="H18" s="6">
-        <f>H17/B19/B1</f>
-        <v>40</v>
-      </c>
+      <c r="G18" s="2"/>
+      <c r="H18" s="6"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B19" s="10">
-        <f>B17+B18</f>
-        <v>27</v>
+        <f>B7-B5-B3</f>
+        <v>20</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H19" s="6">
+        <f>H14-E14</f>
+        <v>5365</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B20" s="10">
-        <f>SUM(B16:B18)</f>
-        <v>30</v>
+        <f>B8-B6-B4</f>
+        <v>7</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H20" s="6">
+        <f>H19/B21/B1</f>
+        <v>39.74074074074074</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" s="10"/>
-      <c r="B21" s="10"/>
+      <c r="A21" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="10">
+        <f>B19+B20</f>
+        <v>27</v>
+      </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" s="10">
+        <f>SUM(B18:B20)</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="10"/>
+      <c r="B23" s="10"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B22" s="11">
+      <c r="B24" s="11">
         <f>SUM(E6:E8)</f>
         <v>1570</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D24" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E22" s="3">
+      <c r="E24" s="3">
         <f>SUM(E3:E4,E6,E7)+B14</f>
         <v>10835</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" s="10" t="s">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="B23" s="11">
+      <c r="B25" s="11">
         <f>SUM(E9:E12)</f>
-        <v>775</v>
-      </c>
-      <c r="D23" s="2" t="s">
+        <v>675</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E23" s="3">
+      <c r="E25" s="3">
         <f>SUM(E5,E8)</f>
         <v>4500</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" s="10"/>
-      <c r="B24" s="10"/>
-      <c r="D24" s="2" t="s">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="10"/>
+      <c r="B26" s="10"/>
+      <c r="D26" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E24" s="5">
-        <f>SUM(E22:E23)</f>
+      <c r="E26" s="5">
+        <f>SUM(E24:E25)</f>
         <v>15335</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" s="10" t="s">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B25" s="11">
-        <f>E3/B17+E5/B19+B22/B19+B23/B19+B13*B1</f>
-        <v>749.35185185185185</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" s="10" t="s">
+      <c r="B27" s="11">
+        <f>E3/B19+E5/B21+B24/B21+B25/B21+B13*B1</f>
+        <v>745.64814814814815</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B26" s="11">
-        <f>E4/B18+E5/B19+B22/B19+B23/B19+B13*B1</f>
-        <v>931.85185185185185</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
+      <c r="B28" s="11">
+        <f>E4/B20+E5/B21+B24/B21+B25/B21+B13*B1</f>
+        <v>928.14814814814815</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B27" s="9">
+      <c r="B29" s="9">
         <v>750</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="2" t="s">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B28" s="9">
+      <c r="B30" s="9">
         <v>930</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>